<commit_message>
Updated gantt chart, more EDA in jisc.ipynb, progress made in project plan report
</commit_message>
<xml_diff>
--- a/documents/Gantt chart.xlsx
+++ b/documents/Gantt chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/425b9db2548ee741/UoB/Data Science Project/MScProject2025-Ali-Suhail/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="169" documentId="8_{A9045851-F1DA-4FAC-92A4-066E2532B652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1167C31-68B4-400E-8986-6EBEF954C34D}"/>
+  <xr:revisionPtr revIDLastSave="246" documentId="8_{A9045851-F1DA-4FAC-92A4-066E2532B652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E34F55F8-E08F-40F3-9DF2-0E37DCA1658B}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-3750" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project schedule" sheetId="11" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
   <si>
     <t>Insert new rows ABOVE this one</t>
   </si>
@@ -113,9 +113,6 @@
     <t xml:space="preserve">Do not delete this row. This row is hidden to preserve a formula that is used to highlight the current day within the project schedule. </t>
   </si>
   <si>
-    <t>Initiation</t>
-  </si>
-  <si>
     <t>Project start:</t>
   </si>
   <si>
@@ -137,15 +134,9 @@
     <t>Data Exploration and Preprocessing</t>
   </si>
   <si>
-    <t>Data Exporation (EDA)</t>
-  </si>
-  <si>
     <t>Establish Machine Learning (ML) Pipeline</t>
   </si>
   <si>
-    <t>Identify risks (MoSCoW)</t>
-  </si>
-  <si>
     <t>Model Development &amp; Evaluation</t>
   </si>
   <si>
@@ -198,6 +189,30 @@
   </si>
   <si>
     <t>Write Future Work (Optional)</t>
+  </si>
+  <si>
+    <t>Must Have</t>
+  </si>
+  <si>
+    <t>PRIORITY</t>
+  </si>
+  <si>
+    <t>Should Have</t>
+  </si>
+  <si>
+    <t>Real-time Dropout Prediction Dashboard</t>
+  </si>
+  <si>
+    <t>Could Have</t>
+  </si>
+  <si>
+    <t>Gantt Chart &amp; Identify Risks (MoSCoW)</t>
+  </si>
+  <si>
+    <t>Project Initiation</t>
+  </si>
+  <si>
+    <t>Exploratory Data Analysis (EDA)</t>
   </si>
 </sst>
 </file>
@@ -782,7 +797,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1063,6 +1078,33 @@
     <xf numFmtId="169" fontId="17" fillId="10" borderId="9" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="17" fillId="10" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="17" fillId="5" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="167" fontId="17" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1080,10 +1122,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="25" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1098,28 +1147,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="25" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="17" fillId="10" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1513,6 +1540,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1722,14 +1753,14 @@
   <dimension ref="A1:BL37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="X16" sqref="X16"/>
+      <selection activeCell="C5" sqref="C5:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.69921875" style="13" customWidth="1"/>
     <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.69921875" customWidth="1"/>
+    <col min="3" max="3" width="16.8984375" customWidth="1"/>
     <col min="4" max="4" width="10.69921875" customWidth="1"/>
     <col min="5" max="5" width="10.69921875" style="2" customWidth="1"/>
     <col min="6" max="6" width="10.69921875" customWidth="1"/>
@@ -1740,70 +1771,70 @@
   <sheetData>
     <row r="1" spans="1:64" ht="53.4" customHeight="1" x14ac:dyDescent="0.8">
       <c r="A1" s="14"/>
-      <c r="B1" s="116" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
+      <c r="B1" s="120" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="107" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" s="108"/>
-      <c r="K1" s="108"/>
-      <c r="L1" s="108"/>
-      <c r="M1" s="108"/>
-      <c r="N1" s="108"/>
-      <c r="O1" s="108"/>
+      <c r="I1" s="118" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="119"/>
+      <c r="K1" s="119"/>
+      <c r="L1" s="119"/>
+      <c r="M1" s="119"/>
+      <c r="N1" s="119"/>
+      <c r="O1" s="119"/>
       <c r="P1" s="20"/>
-      <c r="Q1" s="114">
+      <c r="Q1" s="116">
         <f>DATE(2025, 6, 2)</f>
         <v>45810</v>
       </c>
-      <c r="R1" s="115"/>
-      <c r="S1" s="115"/>
-      <c r="T1" s="115"/>
-      <c r="U1" s="115"/>
-      <c r="V1" s="115"/>
-      <c r="W1" s="115"/>
-      <c r="X1" s="115"/>
-      <c r="Y1" s="115"/>
-      <c r="Z1" s="115"/>
+      <c r="R1" s="117"/>
+      <c r="S1" s="117"/>
+      <c r="T1" s="117"/>
+      <c r="U1" s="117"/>
+      <c r="V1" s="117"/>
+      <c r="W1" s="117"/>
+      <c r="X1" s="117"/>
+      <c r="Y1" s="117"/>
+      <c r="Z1" s="117"/>
     </row>
     <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B2" s="117" t="s">
-        <v>23</v>
+      <c r="B2" s="100" t="s">
+        <v>22</v>
       </c>
       <c r="C2" s="81" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" s="18"/>
       <c r="E2" s="19"/>
       <c r="F2" s="18"/>
-      <c r="I2" s="107" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="108"/>
-      <c r="K2" s="108"/>
-      <c r="L2" s="108"/>
-      <c r="M2" s="108"/>
-      <c r="N2" s="108"/>
-      <c r="O2" s="108"/>
+      <c r="I2" s="118" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="119"/>
+      <c r="K2" s="119"/>
+      <c r="L2" s="119"/>
+      <c r="M2" s="119"/>
+      <c r="N2" s="119"/>
+      <c r="O2" s="119"/>
       <c r="P2" s="20"/>
-      <c r="Q2" s="105">
+      <c r="Q2" s="114">
         <v>1</v>
       </c>
-      <c r="R2" s="106"/>
-      <c r="S2" s="106"/>
-      <c r="T2" s="106"/>
-      <c r="U2" s="106"/>
-      <c r="V2" s="106"/>
-      <c r="W2" s="106"/>
-      <c r="X2" s="106"/>
-      <c r="Y2" s="106"/>
-      <c r="Z2" s="106"/>
+      <c r="R2" s="115"/>
+      <c r="S2" s="115"/>
+      <c r="T2" s="115"/>
+      <c r="U2" s="115"/>
+      <c r="V2" s="115"/>
+      <c r="W2" s="115"/>
+      <c r="X2" s="115"/>
+      <c r="Y2" s="115"/>
+      <c r="Z2" s="115"/>
     </row>
     <row r="3" spans="1:64" s="22" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
@@ -1815,100 +1846,102 @@
       <c r="A4" s="14"/>
       <c r="B4" s="25"/>
       <c r="E4" s="26"/>
-      <c r="I4" s="102">
+      <c r="I4" s="111">
         <f>I5</f>
         <v>45810</v>
       </c>
-      <c r="J4" s="100"/>
-      <c r="K4" s="100"/>
-      <c r="L4" s="100"/>
-      <c r="M4" s="100"/>
-      <c r="N4" s="100"/>
-      <c r="O4" s="100"/>
-      <c r="P4" s="100">
+      <c r="J4" s="109"/>
+      <c r="K4" s="109"/>
+      <c r="L4" s="109"/>
+      <c r="M4" s="109"/>
+      <c r="N4" s="109"/>
+      <c r="O4" s="109"/>
+      <c r="P4" s="109">
         <f>P5</f>
         <v>45817</v>
       </c>
-      <c r="Q4" s="100"/>
-      <c r="R4" s="100"/>
-      <c r="S4" s="100"/>
-      <c r="T4" s="100"/>
-      <c r="U4" s="100"/>
-      <c r="V4" s="100"/>
-      <c r="W4" s="100">
+      <c r="Q4" s="109"/>
+      <c r="R4" s="109"/>
+      <c r="S4" s="109"/>
+      <c r="T4" s="109"/>
+      <c r="U4" s="109"/>
+      <c r="V4" s="109"/>
+      <c r="W4" s="109">
         <f>W5</f>
         <v>45824</v>
       </c>
-      <c r="X4" s="100"/>
-      <c r="Y4" s="100"/>
-      <c r="Z4" s="100"/>
-      <c r="AA4" s="100"/>
-      <c r="AB4" s="100"/>
-      <c r="AC4" s="100"/>
-      <c r="AD4" s="100">
+      <c r="X4" s="109"/>
+      <c r="Y4" s="109"/>
+      <c r="Z4" s="109"/>
+      <c r="AA4" s="109"/>
+      <c r="AB4" s="109"/>
+      <c r="AC4" s="109"/>
+      <c r="AD4" s="109">
         <f>AD5</f>
         <v>45831</v>
       </c>
-      <c r="AE4" s="100"/>
-      <c r="AF4" s="100"/>
-      <c r="AG4" s="100"/>
-      <c r="AH4" s="100"/>
-      <c r="AI4" s="100"/>
-      <c r="AJ4" s="100"/>
-      <c r="AK4" s="100">
+      <c r="AE4" s="109"/>
+      <c r="AF4" s="109"/>
+      <c r="AG4" s="109"/>
+      <c r="AH4" s="109"/>
+      <c r="AI4" s="109"/>
+      <c r="AJ4" s="109"/>
+      <c r="AK4" s="109">
         <f>AK5</f>
         <v>45838</v>
       </c>
-      <c r="AL4" s="100"/>
-      <c r="AM4" s="100"/>
-      <c r="AN4" s="100"/>
-      <c r="AO4" s="100"/>
-      <c r="AP4" s="100"/>
-      <c r="AQ4" s="100"/>
-      <c r="AR4" s="100">
+      <c r="AL4" s="109"/>
+      <c r="AM4" s="109"/>
+      <c r="AN4" s="109"/>
+      <c r="AO4" s="109"/>
+      <c r="AP4" s="109"/>
+      <c r="AQ4" s="109"/>
+      <c r="AR4" s="109">
         <f>AR5</f>
         <v>45845</v>
       </c>
-      <c r="AS4" s="100"/>
-      <c r="AT4" s="100"/>
-      <c r="AU4" s="100"/>
-      <c r="AV4" s="100"/>
-      <c r="AW4" s="100"/>
-      <c r="AX4" s="100"/>
-      <c r="AY4" s="100">
+      <c r="AS4" s="109"/>
+      <c r="AT4" s="109"/>
+      <c r="AU4" s="109"/>
+      <c r="AV4" s="109"/>
+      <c r="AW4" s="109"/>
+      <c r="AX4" s="109"/>
+      <c r="AY4" s="109">
         <f>AY5</f>
         <v>45852</v>
       </c>
-      <c r="AZ4" s="100"/>
-      <c r="BA4" s="100"/>
-      <c r="BB4" s="100"/>
-      <c r="BC4" s="100"/>
-      <c r="BD4" s="100"/>
-      <c r="BE4" s="100"/>
-      <c r="BF4" s="100">
+      <c r="AZ4" s="109"/>
+      <c r="BA4" s="109"/>
+      <c r="BB4" s="109"/>
+      <c r="BC4" s="109"/>
+      <c r="BD4" s="109"/>
+      <c r="BE4" s="109"/>
+      <c r="BF4" s="109">
         <f>BF5</f>
         <v>45859</v>
       </c>
-      <c r="BG4" s="100"/>
-      <c r="BH4" s="100"/>
-      <c r="BI4" s="100"/>
-      <c r="BJ4" s="100"/>
-      <c r="BK4" s="100"/>
-      <c r="BL4" s="101"/>
+      <c r="BG4" s="109"/>
+      <c r="BH4" s="109"/>
+      <c r="BI4" s="109"/>
+      <c r="BJ4" s="109"/>
+      <c r="BK4" s="109"/>
+      <c r="BL4" s="110"/>
     </row>
     <row r="5" spans="1:64" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="109"/>
-      <c r="B5" s="110" t="s">
+      <c r="A5" s="121"/>
+      <c r="B5" s="122" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="112"/>
-      <c r="D5" s="103" t="s">
+      <c r="C5" s="124" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="112" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="103" t="s">
+      <c r="E5" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="103" t="s">
+      <c r="F5" s="112" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="27">
@@ -2137,12 +2170,12 @@
       </c>
     </row>
     <row r="6" spans="1:64" s="22" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="109"/>
-      <c r="B6" s="111"/>
-      <c r="C6" s="113"/>
-      <c r="D6" s="104"/>
-      <c r="E6" s="104"/>
-      <c r="F6" s="104"/>
+      <c r="A6" s="121"/>
+      <c r="B6" s="123"/>
+      <c r="C6" s="125"/>
+      <c r="D6" s="113"/>
+      <c r="E6" s="113"/>
+      <c r="F6" s="113"/>
       <c r="I6" s="30" t="str">
         <f t="shared" ref="I6:AN6" si="3">LEFT(TEXT(I5,"ddd"),1)</f>
         <v>M</v>
@@ -2441,7 +2474,7 @@
     <row r="8" spans="1:64" s="42" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="36" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="C8" s="37"/>
       <c r="D8" s="38"/>
@@ -2512,9 +2545,11 @@
     <row r="9" spans="1:64" s="42" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="44"/>
+        <v>42</v>
+      </c>
+      <c r="C9" s="44" t="s">
+        <v>46</v>
+      </c>
       <c r="D9" s="45">
         <v>1</v>
       </c>
@@ -2591,11 +2626,13 @@
     <row r="10" spans="1:64" s="42" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="48"/>
+        <v>51</v>
+      </c>
+      <c r="C10" s="48" t="s">
+        <v>46</v>
+      </c>
       <c r="D10" s="49">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="E10" s="90">
         <f>F9</f>
@@ -2670,9 +2707,11 @@
     <row r="11" spans="1:64" s="42" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13"/>
       <c r="B11" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="48"/>
+        <v>30</v>
+      </c>
+      <c r="C11" s="48" t="s">
+        <v>46</v>
+      </c>
       <c r="D11" s="49">
         <v>1</v>
       </c>
@@ -2747,9 +2786,11 @@
     <row r="12" spans="1:64" s="42" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13"/>
       <c r="B12" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="48"/>
       <c r="D12" s="49">
         <v>1</v>
       </c>
@@ -2824,11 +2865,13 @@
     <row r="13" spans="1:64" s="42" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13"/>
       <c r="B13" s="47" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="48"/>
+        <v>25</v>
+      </c>
+      <c r="C13" s="48" t="s">
+        <v>46</v>
+      </c>
       <c r="D13" s="49">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="E13" s="90">
         <v>45818</v>
@@ -2901,7 +2944,7 @@
     <row r="14" spans="1:64" s="42" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="51" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" s="52"/>
       <c r="D14" s="53"/>
@@ -2916,9 +2959,11 @@
     <row r="15" spans="1:64" s="42" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="54" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="55"/>
+        <v>53</v>
+      </c>
+      <c r="C15" s="55" t="s">
+        <v>46</v>
+      </c>
       <c r="D15" s="56">
         <v>0.44</v>
       </c>
@@ -2993,9 +3038,11 @@
     <row r="16" spans="1:64" s="42" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="13"/>
       <c r="B16" s="54" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="55"/>
+        <v>29</v>
+      </c>
+      <c r="C16" s="55" t="s">
+        <v>46</v>
+      </c>
       <c r="D16" s="56">
         <v>0</v>
       </c>
@@ -3070,9 +3117,11 @@
     <row r="17" spans="1:64" s="42" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13"/>
       <c r="B17" s="54" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="55"/>
+        <v>27</v>
+      </c>
+      <c r="C17" s="55" t="s">
+        <v>46</v>
+      </c>
       <c r="D17" s="56">
         <v>0</v>
       </c>
@@ -3080,12 +3129,12 @@
         <v>45830</v>
       </c>
       <c r="F17" s="93">
-        <v>45833</v>
+        <v>45832</v>
       </c>
       <c r="G17" s="17"/>
       <c r="H17" s="5">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I17" s="46"/>
       <c r="J17" s="46"/>
@@ -3147,9 +3196,11 @@
     <row r="18" spans="1:64" s="42" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13"/>
       <c r="B18" s="54" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="55"/>
+        <v>31</v>
+      </c>
+      <c r="C18" s="55" t="s">
+        <v>46</v>
+      </c>
       <c r="D18" s="56">
         <v>0</v>
       </c>
@@ -3224,9 +3275,11 @@
     <row r="19" spans="1:64" s="42" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13"/>
       <c r="B19" s="54" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="55"/>
+        <v>32</v>
+      </c>
+      <c r="C19" s="55" t="s">
+        <v>48</v>
+      </c>
       <c r="D19" s="56">
         <v>0</v>
       </c>
@@ -3301,7 +3354,7 @@
     <row r="20" spans="1:64" s="42" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13"/>
       <c r="B20" s="57" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C20" s="58"/>
       <c r="D20" s="59"/>
@@ -3372,19 +3425,19 @@
     <row r="21" spans="1:64" s="42" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13"/>
       <c r="B21" s="61" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="62"/>
+        <v>34</v>
+      </c>
+      <c r="C21" s="62" t="s">
+        <v>46</v>
+      </c>
       <c r="D21" s="63">
         <v>0</v>
       </c>
       <c r="E21" s="96">
-        <f>E9+15</f>
-        <v>45825</v>
+        <v>45838</v>
       </c>
       <c r="F21" s="96">
-        <f>E21+5</f>
-        <v>45830</v>
+        <v>45843</v>
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="5">
@@ -3451,24 +3504,24 @@
     <row r="22" spans="1:64" s="42" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13"/>
       <c r="B22" s="61" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="62"/>
+        <v>33</v>
+      </c>
+      <c r="C22" s="62" t="s">
+        <v>48</v>
+      </c>
       <c r="D22" s="63">
         <v>0</v>
       </c>
       <c r="E22" s="96">
-        <f>F21+1</f>
-        <v>45831</v>
+        <v>45844</v>
       </c>
       <c r="F22" s="96">
-        <f>E22+4</f>
-        <v>45835</v>
+        <v>45850</v>
       </c>
       <c r="G22" s="17"/>
       <c r="H22" s="5">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I22" s="46"/>
       <c r="J22" s="46"/>
@@ -3530,24 +3583,24 @@
     <row r="23" spans="1:64" s="42" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13"/>
       <c r="B23" s="61" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="62"/>
+        <v>35</v>
+      </c>
+      <c r="C23" s="62" t="s">
+        <v>46</v>
+      </c>
       <c r="D23" s="63">
         <v>0</v>
       </c>
       <c r="E23" s="96">
-        <f>E22+5</f>
-        <v>45836</v>
+        <v>45851</v>
       </c>
       <c r="F23" s="96">
-        <f>E23+5</f>
-        <v>45841</v>
+        <v>45855</v>
       </c>
       <c r="G23" s="17"/>
       <c r="H23" s="5">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I23" s="46"/>
       <c r="J23" s="46"/>
@@ -3609,24 +3662,24 @@
     <row r="24" spans="1:64" s="42" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="13"/>
       <c r="B24" s="61" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" s="62"/>
+        <v>36</v>
+      </c>
+      <c r="C24" s="62" t="s">
+        <v>46</v>
+      </c>
       <c r="D24" s="63">
         <v>0</v>
       </c>
       <c r="E24" s="96">
-        <f>F23+1</f>
-        <v>45842</v>
+        <v>45856</v>
       </c>
       <c r="F24" s="96">
-        <f>E24+4</f>
-        <v>45846</v>
+        <v>45862</v>
       </c>
       <c r="G24" s="17"/>
       <c r="H24" s="5">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I24" s="46"/>
       <c r="J24" s="46"/>
@@ -3687,85 +3740,84 @@
     </row>
     <row r="25" spans="1:64" s="42" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13"/>
-      <c r="B25" s="61"/>
-      <c r="C25" s="62"/>
-      <c r="D25" s="63">
+      <c r="B25" s="105" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="106" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="107">
         <v>0</v>
       </c>
-      <c r="E25" s="96">
-        <f>E23</f>
-        <v>45836</v>
-      </c>
-      <c r="F25" s="96">
-        <f>E25+4</f>
-        <v>45840</v>
+      <c r="E25" s="108">
+        <v>45862</v>
+      </c>
+      <c r="F25" s="108">
+        <v>45866</v>
       </c>
       <c r="G25" s="17"/>
-      <c r="H25" s="5">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="I25" s="46"/>
-      <c r="J25" s="46"/>
-      <c r="K25" s="46"/>
-      <c r="L25" s="46"/>
-      <c r="M25" s="46"/>
-      <c r="N25" s="46"/>
-      <c r="O25" s="46"/>
-      <c r="P25" s="46"/>
-      <c r="Q25" s="46"/>
-      <c r="R25" s="46"/>
-      <c r="S25" s="46"/>
-      <c r="T25" s="46"/>
-      <c r="U25" s="46"/>
-      <c r="V25" s="46"/>
-      <c r="W25" s="46"/>
-      <c r="X25" s="46"/>
-      <c r="Y25" s="46"/>
-      <c r="Z25" s="46"/>
-      <c r="AA25" s="46"/>
-      <c r="AB25" s="46"/>
-      <c r="AC25" s="46"/>
-      <c r="AD25" s="46"/>
-      <c r="AE25" s="46"/>
-      <c r="AF25" s="46"/>
-      <c r="AG25" s="46"/>
-      <c r="AH25" s="46"/>
-      <c r="AI25" s="46"/>
-      <c r="AJ25" s="46"/>
-      <c r="AK25" s="46"/>
-      <c r="AL25" s="46"/>
-      <c r="AM25" s="46"/>
-      <c r="AN25" s="46"/>
-      <c r="AO25" s="46"/>
-      <c r="AP25" s="46"/>
-      <c r="AQ25" s="46"/>
-      <c r="AR25" s="46"/>
-      <c r="AS25" s="46"/>
-      <c r="AT25" s="46"/>
-      <c r="AU25" s="46"/>
-      <c r="AV25" s="46"/>
-      <c r="AW25" s="46"/>
-      <c r="AX25" s="46"/>
-      <c r="AY25" s="46"/>
-      <c r="AZ25" s="46"/>
-      <c r="BA25" s="46"/>
-      <c r="BB25" s="46"/>
-      <c r="BC25" s="46"/>
-      <c r="BD25" s="46"/>
-      <c r="BE25" s="46"/>
-      <c r="BF25" s="46"/>
-      <c r="BG25" s="46"/>
-      <c r="BH25" s="46"/>
-      <c r="BI25" s="46"/>
-      <c r="BJ25" s="46"/>
-      <c r="BK25" s="46"/>
-      <c r="BL25" s="46"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="67"/>
+      <c r="J25" s="67"/>
+      <c r="K25" s="67"/>
+      <c r="L25" s="67"/>
+      <c r="M25" s="67"/>
+      <c r="N25" s="67"/>
+      <c r="O25" s="67"/>
+      <c r="P25" s="67"/>
+      <c r="Q25" s="67"/>
+      <c r="R25" s="67"/>
+      <c r="S25" s="67"/>
+      <c r="T25" s="67"/>
+      <c r="U25" s="67"/>
+      <c r="V25" s="67"/>
+      <c r="W25" s="67"/>
+      <c r="X25" s="67"/>
+      <c r="Y25" s="67"/>
+      <c r="Z25" s="67"/>
+      <c r="AA25" s="67"/>
+      <c r="AB25" s="67"/>
+      <c r="AC25" s="67"/>
+      <c r="AD25" s="67"/>
+      <c r="AE25" s="67"/>
+      <c r="AF25" s="67"/>
+      <c r="AG25" s="67"/>
+      <c r="AH25" s="67"/>
+      <c r="AI25" s="67"/>
+      <c r="AJ25" s="67"/>
+      <c r="AK25" s="67"/>
+      <c r="AL25" s="67"/>
+      <c r="AM25" s="67"/>
+      <c r="AN25" s="67"/>
+      <c r="AO25" s="67"/>
+      <c r="AP25" s="67"/>
+      <c r="AQ25" s="67"/>
+      <c r="AR25" s="67"/>
+      <c r="AS25" s="67"/>
+      <c r="AT25" s="67"/>
+      <c r="AU25" s="67"/>
+      <c r="AV25" s="67"/>
+      <c r="AW25" s="67"/>
+      <c r="AX25" s="67"/>
+      <c r="AY25" s="67"/>
+      <c r="AZ25" s="67"/>
+      <c r="BA25" s="67"/>
+      <c r="BB25" s="67"/>
+      <c r="BC25" s="67"/>
+      <c r="BD25" s="67"/>
+      <c r="BE25" s="67"/>
+      <c r="BF25" s="67"/>
+      <c r="BG25" s="67"/>
+      <c r="BH25" s="67"/>
+      <c r="BI25" s="67"/>
+      <c r="BJ25" s="67"/>
+      <c r="BK25" s="67"/>
+      <c r="BL25" s="67"/>
     </row>
     <row r="26" spans="1:64" s="42" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="13"/>
       <c r="B26" s="64" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C26" s="65"/>
       <c r="D26" s="66"/>
@@ -3836,22 +3888,24 @@
     <row r="27" spans="1:64" s="42" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="13"/>
       <c r="B27" s="68" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="69"/>
+        <v>38</v>
+      </c>
+      <c r="C27" s="69" t="s">
+        <v>46</v>
+      </c>
       <c r="D27" s="70">
         <v>0</v>
       </c>
       <c r="E27" s="99">
-        <v>45884</v>
+        <v>45863</v>
       </c>
       <c r="F27" s="99">
-        <v>45900</v>
+        <v>45869</v>
       </c>
       <c r="G27" s="17"/>
       <c r="H27" s="5">
         <f t="shared" si="5"/>
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="I27" s="46"/>
       <c r="J27" s="46"/>
@@ -3913,22 +3967,24 @@
     <row r="28" spans="1:64" s="42" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="13"/>
       <c r="B28" s="68" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" s="69"/>
+        <v>39</v>
+      </c>
+      <c r="C28" s="69" t="s">
+        <v>46</v>
+      </c>
       <c r="D28" s="70">
         <v>0</v>
       </c>
       <c r="E28" s="99">
-        <v>45884</v>
+        <v>45870</v>
       </c>
       <c r="F28" s="99">
-        <v>45900</v>
+        <v>45876</v>
       </c>
       <c r="G28" s="17"/>
       <c r="H28" s="5">
         <f t="shared" si="5"/>
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="I28" s="46"/>
       <c r="J28" s="46"/>
@@ -3990,22 +4046,24 @@
     <row r="29" spans="1:64" s="42" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="13"/>
       <c r="B29" s="68" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" s="69"/>
+        <v>40</v>
+      </c>
+      <c r="C29" s="69" t="s">
+        <v>46</v>
+      </c>
       <c r="D29" s="70">
         <v>0</v>
       </c>
       <c r="E29" s="99">
-        <v>45884</v>
+        <v>45877</v>
       </c>
       <c r="F29" s="99">
-        <v>45900</v>
+        <v>45883</v>
       </c>
       <c r="G29" s="17"/>
       <c r="H29" s="5">
         <f t="shared" si="5"/>
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="I29" s="46"/>
       <c r="J29" s="46"/>
@@ -4067,9 +4125,11 @@
     <row r="30" spans="1:64" s="42" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13"/>
       <c r="B30" s="68" t="s">
-        <v>47</v>
-      </c>
-      <c r="C30" s="69"/>
+        <v>44</v>
+      </c>
+      <c r="C30" s="69" t="s">
+        <v>46</v>
+      </c>
       <c r="D30" s="70">
         <v>0</v>
       </c>
@@ -4077,12 +4137,12 @@
         <v>45884</v>
       </c>
       <c r="F30" s="99">
-        <v>45900</v>
+        <v>45890</v>
       </c>
       <c r="G30" s="17"/>
       <c r="H30" s="5">
         <f t="shared" si="5"/>
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="I30" s="46"/>
       <c r="J30" s="46"/>
@@ -4144,22 +4204,24 @@
     <row r="31" spans="1:64" s="42" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="13"/>
       <c r="B31" s="68" t="s">
-        <v>48</v>
-      </c>
-      <c r="C31" s="69"/>
+        <v>45</v>
+      </c>
+      <c r="C31" s="69" t="s">
+        <v>50</v>
+      </c>
       <c r="D31" s="70">
         <v>0</v>
       </c>
       <c r="E31" s="99">
-        <v>45884</v>
+        <v>45886</v>
       </c>
       <c r="F31" s="99">
-        <v>45900</v>
+        <v>45890</v>
       </c>
       <c r="G31" s="17"/>
       <c r="H31" s="5">
         <f t="shared" si="5"/>
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="I31" s="46"/>
       <c r="J31" s="46"/>
@@ -4220,15 +4282,21 @@
     </row>
     <row r="32" spans="1:64" s="42" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="13"/>
-      <c r="B32" s="118" t="s">
-        <v>44</v>
-      </c>
-      <c r="C32" s="119"/>
-      <c r="D32" s="120">
+      <c r="B32" s="101" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="102" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" s="103">
         <v>0</v>
       </c>
-      <c r="E32" s="121"/>
-      <c r="F32" s="121"/>
+      <c r="E32" s="104">
+        <v>45891</v>
+      </c>
+      <c r="F32" s="104">
+        <v>45896</v>
+      </c>
       <c r="G32" s="17"/>
       <c r="H32" s="5"/>
       <c r="I32" s="41"/>
@@ -4511,7 +4579,7 @@
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="13">
+  <dataValidations count="13">
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Changing this number will scroll the Gantt Chart view." sqref="Q2" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>1</formula1>
     </dataValidation>
@@ -4534,9 +4602,6 @@
   <headerFooter differentFirst="1" scaleWithDoc="0">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
-  <ignoredErrors>
-    <ignoredError sqref="F22:F23 E23" formula="1"/>
-  </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>

</xml_diff>

<commit_message>
Finished processing summarised dataset
</commit_message>
<xml_diff>
--- a/documents/Gantt chart.xlsx
+++ b/documents/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/425b9db2548ee741/UoB/Data Science Project/MScProject2025-Ali-Suhail/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="246" documentId="8_{A9045851-F1DA-4FAC-92A4-066E2532B652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E34F55F8-E08F-40F3-9DF2-0E37DCA1658B}"/>
+  <xr:revisionPtr revIDLastSave="251" documentId="8_{A9045851-F1DA-4FAC-92A4-066E2532B652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CAB533CD-AC7A-4104-A4E8-D5352D299E9D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1105,14 +1105,20 @@
     <xf numFmtId="169" fontId="17" fillId="5" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="17" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="17" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="17" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1133,20 +1139,14 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="167" fontId="17" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1752,8 +1752,8 @@
   </sheetPr>
   <dimension ref="A1:BL37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C6"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A3" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1771,37 +1771,37 @@
   <sheetData>
     <row r="1" spans="1:64" ht="53.4" customHeight="1" x14ac:dyDescent="0.8">
       <c r="A1" s="14"/>
-      <c r="B1" s="120" t="s">
+      <c r="B1" s="122" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="118" t="s">
+      <c r="I1" s="120" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="119"/>
-      <c r="K1" s="119"/>
-      <c r="L1" s="119"/>
-      <c r="M1" s="119"/>
-      <c r="N1" s="119"/>
-      <c r="O1" s="119"/>
+      <c r="J1" s="121"/>
+      <c r="K1" s="121"/>
+      <c r="L1" s="121"/>
+      <c r="M1" s="121"/>
+      <c r="N1" s="121"/>
+      <c r="O1" s="121"/>
       <c r="P1" s="20"/>
-      <c r="Q1" s="116">
+      <c r="Q1" s="118">
         <f>DATE(2025, 6, 2)</f>
         <v>45810</v>
       </c>
-      <c r="R1" s="117"/>
-      <c r="S1" s="117"/>
-      <c r="T1" s="117"/>
-      <c r="U1" s="117"/>
-      <c r="V1" s="117"/>
-      <c r="W1" s="117"/>
-      <c r="X1" s="117"/>
-      <c r="Y1" s="117"/>
-      <c r="Z1" s="117"/>
+      <c r="R1" s="119"/>
+      <c r="S1" s="119"/>
+      <c r="T1" s="119"/>
+      <c r="U1" s="119"/>
+      <c r="V1" s="119"/>
+      <c r="W1" s="119"/>
+      <c r="X1" s="119"/>
+      <c r="Y1" s="119"/>
+      <c r="Z1" s="119"/>
     </row>
     <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B2" s="100" t="s">
@@ -1813,28 +1813,28 @@
       <c r="D2" s="18"/>
       <c r="E2" s="19"/>
       <c r="F2" s="18"/>
-      <c r="I2" s="118" t="s">
+      <c r="I2" s="120" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="119"/>
-      <c r="K2" s="119"/>
-      <c r="L2" s="119"/>
-      <c r="M2" s="119"/>
-      <c r="N2" s="119"/>
-      <c r="O2" s="119"/>
+      <c r="J2" s="121"/>
+      <c r="K2" s="121"/>
+      <c r="L2" s="121"/>
+      <c r="M2" s="121"/>
+      <c r="N2" s="121"/>
+      <c r="O2" s="121"/>
       <c r="P2" s="20"/>
-      <c r="Q2" s="114">
+      <c r="Q2" s="116">
         <v>1</v>
       </c>
-      <c r="R2" s="115"/>
-      <c r="S2" s="115"/>
-      <c r="T2" s="115"/>
-      <c r="U2" s="115"/>
-      <c r="V2" s="115"/>
-      <c r="W2" s="115"/>
-      <c r="X2" s="115"/>
-      <c r="Y2" s="115"/>
-      <c r="Z2" s="115"/>
+      <c r="R2" s="117"/>
+      <c r="S2" s="117"/>
+      <c r="T2" s="117"/>
+      <c r="U2" s="117"/>
+      <c r="V2" s="117"/>
+      <c r="W2" s="117"/>
+      <c r="X2" s="117"/>
+      <c r="Y2" s="117"/>
+      <c r="Z2" s="117"/>
     </row>
     <row r="3" spans="1:64" s="22" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
@@ -1846,102 +1846,102 @@
       <c r="A4" s="14"/>
       <c r="B4" s="25"/>
       <c r="E4" s="26"/>
-      <c r="I4" s="111">
+      <c r="I4" s="125">
         <f>I5</f>
         <v>45810</v>
       </c>
-      <c r="J4" s="109"/>
-      <c r="K4" s="109"/>
-      <c r="L4" s="109"/>
-      <c r="M4" s="109"/>
-      <c r="N4" s="109"/>
-      <c r="O4" s="109"/>
-      <c r="P4" s="109">
+      <c r="J4" s="123"/>
+      <c r="K4" s="123"/>
+      <c r="L4" s="123"/>
+      <c r="M4" s="123"/>
+      <c r="N4" s="123"/>
+      <c r="O4" s="123"/>
+      <c r="P4" s="123">
         <f>P5</f>
         <v>45817</v>
       </c>
-      <c r="Q4" s="109"/>
-      <c r="R4" s="109"/>
-      <c r="S4" s="109"/>
-      <c r="T4" s="109"/>
-      <c r="U4" s="109"/>
-      <c r="V4" s="109"/>
-      <c r="W4" s="109">
+      <c r="Q4" s="123"/>
+      <c r="R4" s="123"/>
+      <c r="S4" s="123"/>
+      <c r="T4" s="123"/>
+      <c r="U4" s="123"/>
+      <c r="V4" s="123"/>
+      <c r="W4" s="123">
         <f>W5</f>
         <v>45824</v>
       </c>
-      <c r="X4" s="109"/>
-      <c r="Y4" s="109"/>
-      <c r="Z4" s="109"/>
-      <c r="AA4" s="109"/>
-      <c r="AB4" s="109"/>
-      <c r="AC4" s="109"/>
-      <c r="AD4" s="109">
+      <c r="X4" s="123"/>
+      <c r="Y4" s="123"/>
+      <c r="Z4" s="123"/>
+      <c r="AA4" s="123"/>
+      <c r="AB4" s="123"/>
+      <c r="AC4" s="123"/>
+      <c r="AD4" s="123">
         <f>AD5</f>
         <v>45831</v>
       </c>
-      <c r="AE4" s="109"/>
-      <c r="AF4" s="109"/>
-      <c r="AG4" s="109"/>
-      <c r="AH4" s="109"/>
-      <c r="AI4" s="109"/>
-      <c r="AJ4" s="109"/>
-      <c r="AK4" s="109">
+      <c r="AE4" s="123"/>
+      <c r="AF4" s="123"/>
+      <c r="AG4" s="123"/>
+      <c r="AH4" s="123"/>
+      <c r="AI4" s="123"/>
+      <c r="AJ4" s="123"/>
+      <c r="AK4" s="123">
         <f>AK5</f>
         <v>45838</v>
       </c>
-      <c r="AL4" s="109"/>
-      <c r="AM4" s="109"/>
-      <c r="AN4" s="109"/>
-      <c r="AO4" s="109"/>
-      <c r="AP4" s="109"/>
-      <c r="AQ4" s="109"/>
-      <c r="AR4" s="109">
+      <c r="AL4" s="123"/>
+      <c r="AM4" s="123"/>
+      <c r="AN4" s="123"/>
+      <c r="AO4" s="123"/>
+      <c r="AP4" s="123"/>
+      <c r="AQ4" s="123"/>
+      <c r="AR4" s="123">
         <f>AR5</f>
         <v>45845</v>
       </c>
-      <c r="AS4" s="109"/>
-      <c r="AT4" s="109"/>
-      <c r="AU4" s="109"/>
-      <c r="AV4" s="109"/>
-      <c r="AW4" s="109"/>
-      <c r="AX4" s="109"/>
-      <c r="AY4" s="109">
+      <c r="AS4" s="123"/>
+      <c r="AT4" s="123"/>
+      <c r="AU4" s="123"/>
+      <c r="AV4" s="123"/>
+      <c r="AW4" s="123"/>
+      <c r="AX4" s="123"/>
+      <c r="AY4" s="123">
         <f>AY5</f>
         <v>45852</v>
       </c>
-      <c r="AZ4" s="109"/>
-      <c r="BA4" s="109"/>
-      <c r="BB4" s="109"/>
-      <c r="BC4" s="109"/>
-      <c r="BD4" s="109"/>
-      <c r="BE4" s="109"/>
-      <c r="BF4" s="109">
+      <c r="AZ4" s="123"/>
+      <c r="BA4" s="123"/>
+      <c r="BB4" s="123"/>
+      <c r="BC4" s="123"/>
+      <c r="BD4" s="123"/>
+      <c r="BE4" s="123"/>
+      <c r="BF4" s="123">
         <f>BF5</f>
         <v>45859</v>
       </c>
-      <c r="BG4" s="109"/>
-      <c r="BH4" s="109"/>
-      <c r="BI4" s="109"/>
-      <c r="BJ4" s="109"/>
-      <c r="BK4" s="109"/>
-      <c r="BL4" s="110"/>
+      <c r="BG4" s="123"/>
+      <c r="BH4" s="123"/>
+      <c r="BI4" s="123"/>
+      <c r="BJ4" s="123"/>
+      <c r="BK4" s="123"/>
+      <c r="BL4" s="124"/>
     </row>
     <row r="5" spans="1:64" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="121"/>
-      <c r="B5" s="122" t="s">
+      <c r="A5" s="109"/>
+      <c r="B5" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="124" t="s">
+      <c r="C5" s="112" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="112" t="s">
+      <c r="D5" s="114" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="112" t="s">
+      <c r="E5" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="112" t="s">
+      <c r="F5" s="114" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="27">
@@ -2170,12 +2170,12 @@
       </c>
     </row>
     <row r="6" spans="1:64" s="22" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="121"/>
-      <c r="B6" s="123"/>
-      <c r="C6" s="125"/>
-      <c r="D6" s="113"/>
-      <c r="E6" s="113"/>
-      <c r="F6" s="113"/>
+      <c r="A6" s="109"/>
+      <c r="B6" s="111"/>
+      <c r="C6" s="113"/>
+      <c r="D6" s="115"/>
+      <c r="E6" s="115"/>
+      <c r="F6" s="115"/>
       <c r="I6" s="30" t="str">
         <f t="shared" ref="I6:AN6" si="3">LEFT(TEXT(I5,"ddd"),1)</f>
         <v>M</v>
@@ -2871,7 +2871,7 @@
         <v>46</v>
       </c>
       <c r="D13" s="49">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="E13" s="90">
         <v>45818</v>
@@ -2965,7 +2965,7 @@
         <v>46</v>
       </c>
       <c r="D15" s="56">
-        <v>0.44</v>
+        <v>0.5</v>
       </c>
       <c r="E15" s="93">
         <v>45822</v>
@@ -3044,7 +3044,7 @@
         <v>46</v>
       </c>
       <c r="D16" s="56">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="E16" s="93">
         <v>45826</v>
@@ -4508,17 +4508,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="Q1:Z1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="B1:F1"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
@@ -4527,6 +4516,17 @@
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="Q1:Z1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D34">
     <cfRule type="dataBar" priority="23">
@@ -4751,35 +4751,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="28" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="60f5a4f2d2b0abadcf532d48ebf9cb71">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7dd78129e6a1811f84807ad11c651531" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5091,10 +5062,52 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2348D59-3426-404A-A0C5-6456F6613EDB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5119,22 +5132,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2348D59-3426-404A-A0C5-6456F6613EDB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fixed bugs and preprocessing errors. Added new notebook file called dropout_dataset_generator, automating task. Updated logs and Gnatt chart
</commit_message>
<xml_diff>
--- a/documents/Gantt chart.xlsx
+++ b/documents/Gantt chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/425b9db2548ee741/UoB/Data Science Project/MScProject2025-Ali-Suhail/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="251" documentId="8_{A9045851-F1DA-4FAC-92A4-066E2532B652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CAB533CD-AC7A-4104-A4E8-D5352D299E9D}"/>
+  <xr:revisionPtr revIDLastSave="255" documentId="8_{A9045851-F1DA-4FAC-92A4-066E2532B652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7E41877-E813-46B3-AC90-B7FAF0E4206E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-3750" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project schedule" sheetId="11" r:id="rId1"/>
@@ -1105,20 +1105,14 @@
     <xf numFmtId="169" fontId="17" fillId="5" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="167" fontId="17" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1139,14 +1133,20 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="17" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="17" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="17" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1752,8 +1752,8 @@
   </sheetPr>
   <dimension ref="A1:BL37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A3" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A11" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1771,37 +1771,37 @@
   <sheetData>
     <row r="1" spans="1:64" ht="53.4" customHeight="1" x14ac:dyDescent="0.8">
       <c r="A1" s="14"/>
-      <c r="B1" s="122" t="s">
+      <c r="B1" s="120" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="120" t="s">
+      <c r="I1" s="118" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="121"/>
-      <c r="K1" s="121"/>
-      <c r="L1" s="121"/>
-      <c r="M1" s="121"/>
-      <c r="N1" s="121"/>
-      <c r="O1" s="121"/>
+      <c r="J1" s="119"/>
+      <c r="K1" s="119"/>
+      <c r="L1" s="119"/>
+      <c r="M1" s="119"/>
+      <c r="N1" s="119"/>
+      <c r="O1" s="119"/>
       <c r="P1" s="20"/>
-      <c r="Q1" s="118">
+      <c r="Q1" s="116">
         <f>DATE(2025, 6, 2)</f>
         <v>45810</v>
       </c>
-      <c r="R1" s="119"/>
-      <c r="S1" s="119"/>
-      <c r="T1" s="119"/>
-      <c r="U1" s="119"/>
-      <c r="V1" s="119"/>
-      <c r="W1" s="119"/>
-      <c r="X1" s="119"/>
-      <c r="Y1" s="119"/>
-      <c r="Z1" s="119"/>
+      <c r="R1" s="117"/>
+      <c r="S1" s="117"/>
+      <c r="T1" s="117"/>
+      <c r="U1" s="117"/>
+      <c r="V1" s="117"/>
+      <c r="W1" s="117"/>
+      <c r="X1" s="117"/>
+      <c r="Y1" s="117"/>
+      <c r="Z1" s="117"/>
     </row>
     <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B2" s="100" t="s">
@@ -1813,28 +1813,28 @@
       <c r="D2" s="18"/>
       <c r="E2" s="19"/>
       <c r="F2" s="18"/>
-      <c r="I2" s="120" t="s">
+      <c r="I2" s="118" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="121"/>
-      <c r="K2" s="121"/>
-      <c r="L2" s="121"/>
-      <c r="M2" s="121"/>
-      <c r="N2" s="121"/>
-      <c r="O2" s="121"/>
+      <c r="J2" s="119"/>
+      <c r="K2" s="119"/>
+      <c r="L2" s="119"/>
+      <c r="M2" s="119"/>
+      <c r="N2" s="119"/>
+      <c r="O2" s="119"/>
       <c r="P2" s="20"/>
-      <c r="Q2" s="116">
+      <c r="Q2" s="114">
         <v>1</v>
       </c>
-      <c r="R2" s="117"/>
-      <c r="S2" s="117"/>
-      <c r="T2" s="117"/>
-      <c r="U2" s="117"/>
-      <c r="V2" s="117"/>
-      <c r="W2" s="117"/>
-      <c r="X2" s="117"/>
-      <c r="Y2" s="117"/>
-      <c r="Z2" s="117"/>
+      <c r="R2" s="115"/>
+      <c r="S2" s="115"/>
+      <c r="T2" s="115"/>
+      <c r="U2" s="115"/>
+      <c r="V2" s="115"/>
+      <c r="W2" s="115"/>
+      <c r="X2" s="115"/>
+      <c r="Y2" s="115"/>
+      <c r="Z2" s="115"/>
     </row>
     <row r="3" spans="1:64" s="22" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
@@ -1846,102 +1846,102 @@
       <c r="A4" s="14"/>
       <c r="B4" s="25"/>
       <c r="E4" s="26"/>
-      <c r="I4" s="125">
+      <c r="I4" s="111">
         <f>I5</f>
         <v>45810</v>
       </c>
-      <c r="J4" s="123"/>
-      <c r="K4" s="123"/>
-      <c r="L4" s="123"/>
-      <c r="M4" s="123"/>
-      <c r="N4" s="123"/>
-      <c r="O4" s="123"/>
-      <c r="P4" s="123">
+      <c r="J4" s="109"/>
+      <c r="K4" s="109"/>
+      <c r="L4" s="109"/>
+      <c r="M4" s="109"/>
+      <c r="N4" s="109"/>
+      <c r="O4" s="109"/>
+      <c r="P4" s="109">
         <f>P5</f>
         <v>45817</v>
       </c>
-      <c r="Q4" s="123"/>
-      <c r="R4" s="123"/>
-      <c r="S4" s="123"/>
-      <c r="T4" s="123"/>
-      <c r="U4" s="123"/>
-      <c r="V4" s="123"/>
-      <c r="W4" s="123">
+      <c r="Q4" s="109"/>
+      <c r="R4" s="109"/>
+      <c r="S4" s="109"/>
+      <c r="T4" s="109"/>
+      <c r="U4" s="109"/>
+      <c r="V4" s="109"/>
+      <c r="W4" s="109">
         <f>W5</f>
         <v>45824</v>
       </c>
-      <c r="X4" s="123"/>
-      <c r="Y4" s="123"/>
-      <c r="Z4" s="123"/>
-      <c r="AA4" s="123"/>
-      <c r="AB4" s="123"/>
-      <c r="AC4" s="123"/>
-      <c r="AD4" s="123">
+      <c r="X4" s="109"/>
+      <c r="Y4" s="109"/>
+      <c r="Z4" s="109"/>
+      <c r="AA4" s="109"/>
+      <c r="AB4" s="109"/>
+      <c r="AC4" s="109"/>
+      <c r="AD4" s="109">
         <f>AD5</f>
         <v>45831</v>
       </c>
-      <c r="AE4" s="123"/>
-      <c r="AF4" s="123"/>
-      <c r="AG4" s="123"/>
-      <c r="AH4" s="123"/>
-      <c r="AI4" s="123"/>
-      <c r="AJ4" s="123"/>
-      <c r="AK4" s="123">
+      <c r="AE4" s="109"/>
+      <c r="AF4" s="109"/>
+      <c r="AG4" s="109"/>
+      <c r="AH4" s="109"/>
+      <c r="AI4" s="109"/>
+      <c r="AJ4" s="109"/>
+      <c r="AK4" s="109">
         <f>AK5</f>
         <v>45838</v>
       </c>
-      <c r="AL4" s="123"/>
-      <c r="AM4" s="123"/>
-      <c r="AN4" s="123"/>
-      <c r="AO4" s="123"/>
-      <c r="AP4" s="123"/>
-      <c r="AQ4" s="123"/>
-      <c r="AR4" s="123">
+      <c r="AL4" s="109"/>
+      <c r="AM4" s="109"/>
+      <c r="AN4" s="109"/>
+      <c r="AO4" s="109"/>
+      <c r="AP4" s="109"/>
+      <c r="AQ4" s="109"/>
+      <c r="AR4" s="109">
         <f>AR5</f>
         <v>45845</v>
       </c>
-      <c r="AS4" s="123"/>
-      <c r="AT4" s="123"/>
-      <c r="AU4" s="123"/>
-      <c r="AV4" s="123"/>
-      <c r="AW4" s="123"/>
-      <c r="AX4" s="123"/>
-      <c r="AY4" s="123">
+      <c r="AS4" s="109"/>
+      <c r="AT4" s="109"/>
+      <c r="AU4" s="109"/>
+      <c r="AV4" s="109"/>
+      <c r="AW4" s="109"/>
+      <c r="AX4" s="109"/>
+      <c r="AY4" s="109">
         <f>AY5</f>
         <v>45852</v>
       </c>
-      <c r="AZ4" s="123"/>
-      <c r="BA4" s="123"/>
-      <c r="BB4" s="123"/>
-      <c r="BC4" s="123"/>
-      <c r="BD4" s="123"/>
-      <c r="BE4" s="123"/>
-      <c r="BF4" s="123">
+      <c r="AZ4" s="109"/>
+      <c r="BA4" s="109"/>
+      <c r="BB4" s="109"/>
+      <c r="BC4" s="109"/>
+      <c r="BD4" s="109"/>
+      <c r="BE4" s="109"/>
+      <c r="BF4" s="109">
         <f>BF5</f>
         <v>45859</v>
       </c>
-      <c r="BG4" s="123"/>
-      <c r="BH4" s="123"/>
-      <c r="BI4" s="123"/>
-      <c r="BJ4" s="123"/>
-      <c r="BK4" s="123"/>
-      <c r="BL4" s="124"/>
+      <c r="BG4" s="109"/>
+      <c r="BH4" s="109"/>
+      <c r="BI4" s="109"/>
+      <c r="BJ4" s="109"/>
+      <c r="BK4" s="109"/>
+      <c r="BL4" s="110"/>
     </row>
     <row r="5" spans="1:64" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="109"/>
-      <c r="B5" s="110" t="s">
+      <c r="A5" s="121"/>
+      <c r="B5" s="122" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="112" t="s">
+      <c r="C5" s="124" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="114" t="s">
+      <c r="D5" s="112" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="114" t="s">
+      <c r="E5" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="114" t="s">
+      <c r="F5" s="112" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="27">
@@ -2170,12 +2170,12 @@
       </c>
     </row>
     <row r="6" spans="1:64" s="22" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="109"/>
-      <c r="B6" s="111"/>
-      <c r="C6" s="113"/>
-      <c r="D6" s="115"/>
-      <c r="E6" s="115"/>
-      <c r="F6" s="115"/>
+      <c r="A6" s="121"/>
+      <c r="B6" s="123"/>
+      <c r="C6" s="125"/>
+      <c r="D6" s="113"/>
+      <c r="E6" s="113"/>
+      <c r="F6" s="113"/>
       <c r="I6" s="30" t="str">
         <f t="shared" ref="I6:AN6" si="3">LEFT(TEXT(I5,"ddd"),1)</f>
         <v>M</v>
@@ -2965,7 +2965,7 @@
         <v>46</v>
       </c>
       <c r="D15" s="56">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E15" s="93">
         <v>45822</v>
@@ -3044,7 +3044,7 @@
         <v>46</v>
       </c>
       <c r="D16" s="56">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="E16" s="93">
         <v>45826</v>
@@ -3123,7 +3123,7 @@
         <v>46</v>
       </c>
       <c r="D17" s="56">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="E17" s="93">
         <v>45830</v>
@@ -3202,7 +3202,7 @@
         <v>46</v>
       </c>
       <c r="D18" s="56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="93">
         <v>45833</v>
@@ -4508,6 +4508,17 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="Q1:Z1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="B1:F1"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
@@ -4516,17 +4527,6 @@
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="Q1:Z1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D34">
     <cfRule type="dataBar" priority="23">
@@ -4751,6 +4751,35 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="28" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="60f5a4f2d2b0abadcf532d48ebf9cb71">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7dd78129e6a1811f84807ad11c651531" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5062,52 +5091,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2348D59-3426-404A-A0C5-6456F6613EDB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5132,9 +5119,22 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2348D59-3426-404A-A0C5-6456F6613EDB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
EDA 95% complete, data scaling partically complete, LR basic model added
</commit_message>
<xml_diff>
--- a/documents/Gantt chart.xlsx
+++ b/documents/Gantt chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/425b9db2548ee741/UoB/Data Science Project/MScProject2025-Ali-Suhail/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="255" documentId="8_{A9045851-F1DA-4FAC-92A4-066E2532B652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7E41877-E813-46B3-AC90-B7FAF0E4206E}"/>
+  <xr:revisionPtr revIDLastSave="261" documentId="8_{A9045851-F1DA-4FAC-92A4-066E2532B652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1967B408-8650-42FA-AA64-E540E6E79142}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-3750" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project schedule" sheetId="11" r:id="rId1"/>
@@ -1753,7 +1753,7 @@
   <dimension ref="A1:BL37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A11" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2965,7 +2965,7 @@
         <v>46</v>
       </c>
       <c r="D15" s="56">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="E15" s="93">
         <v>45822</v>
@@ -3044,7 +3044,7 @@
         <v>46</v>
       </c>
       <c r="D16" s="56">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E16" s="93">
         <v>45826</v>
@@ -3123,7 +3123,7 @@
         <v>46</v>
       </c>
       <c r="D17" s="56">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E17" s="93">
         <v>45830</v>
@@ -3281,7 +3281,7 @@
         <v>48</v>
       </c>
       <c r="D19" s="56">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E19" s="93">
         <v>45835</v>
@@ -3431,7 +3431,7 @@
         <v>46</v>
       </c>
       <c r="D21" s="63">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E21" s="96">
         <v>45838</v>

</xml_diff>

<commit_message>
folder changes, fixed folder feature bug in dropout_dataset_generator.ipynb, Logistic regression model and results completed and added SVM model
</commit_message>
<xml_diff>
--- a/documents/Gantt chart.xlsx
+++ b/documents/Gantt chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/425b9db2548ee741/UoB/Data Science Project/MScProject2025-Ali-Suhail/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="261" documentId="8_{A9045851-F1DA-4FAC-92A4-066E2532B652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1967B408-8650-42FA-AA64-E540E6E79142}"/>
+  <xr:revisionPtr revIDLastSave="272" documentId="8_{A9045851-F1DA-4FAC-92A4-066E2532B652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C65A8C50-FC18-4778-AD14-9FF36B291F4D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1752,8 +1752,8 @@
   </sheetPr>
   <dimension ref="A1:BL37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A11" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A20" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2965,7 +2965,7 @@
         <v>46</v>
       </c>
       <c r="D15" s="56">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="E15" s="93">
         <v>45822</v>
@@ -3281,7 +3281,7 @@
         <v>48</v>
       </c>
       <c r="D19" s="56">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E19" s="93">
         <v>45835</v>
@@ -3431,7 +3431,7 @@
         <v>46</v>
       </c>
       <c r="D21" s="63">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="E21" s="96">
         <v>45838</v>
@@ -3510,7 +3510,7 @@
         <v>48</v>
       </c>
       <c r="D22" s="63">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="E22" s="96">
         <v>45844</v>
@@ -3589,7 +3589,7 @@
         <v>46</v>
       </c>
       <c r="D23" s="63">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="E23" s="96">
         <v>45851</v>
@@ -3668,7 +3668,7 @@
         <v>46</v>
       </c>
       <c r="D24" s="63">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="E24" s="96">
         <v>45856</v>

</xml_diff>

<commit_message>
Added Jisc presentation slides. Implemented, trained and evaluated SVM and MLP models (Partially Completed)
</commit_message>
<xml_diff>
--- a/documents/Gantt chart.xlsx
+++ b/documents/Gantt chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/425b9db2548ee741/UoB/Data Science Project/MScProject2025-Ali-Suhail/documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alisu\OneDrive\UoB\Data Science Project\MScProject2025-Ali-Suhail\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="272" documentId="8_{A9045851-F1DA-4FAC-92A4-066E2532B652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C65A8C50-FC18-4778-AD14-9FF36B291F4D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472B5602-26CD-4C43-A521-B84F06392F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-3750" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project schedule" sheetId="11" r:id="rId1"/>
@@ -1105,14 +1105,20 @@
     <xf numFmtId="169" fontId="17" fillId="5" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="17" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="17" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="17" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1133,20 +1139,14 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="167" fontId="17" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1540,10 +1540,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1752,8 +1748,8 @@
   </sheetPr>
   <dimension ref="A1:BL37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A20" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A11" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="BB23" sqref="BA23:BB23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1771,37 +1767,37 @@
   <sheetData>
     <row r="1" spans="1:64" ht="53.4" customHeight="1" x14ac:dyDescent="0.8">
       <c r="A1" s="14"/>
-      <c r="B1" s="120" t="s">
+      <c r="B1" s="122" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="118" t="s">
+      <c r="I1" s="120" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="119"/>
-      <c r="K1" s="119"/>
-      <c r="L1" s="119"/>
-      <c r="M1" s="119"/>
-      <c r="N1" s="119"/>
-      <c r="O1" s="119"/>
+      <c r="J1" s="121"/>
+      <c r="K1" s="121"/>
+      <c r="L1" s="121"/>
+      <c r="M1" s="121"/>
+      <c r="N1" s="121"/>
+      <c r="O1" s="121"/>
       <c r="P1" s="20"/>
-      <c r="Q1" s="116">
+      <c r="Q1" s="118">
         <f>DATE(2025, 6, 2)</f>
         <v>45810</v>
       </c>
-      <c r="R1" s="117"/>
-      <c r="S1" s="117"/>
-      <c r="T1" s="117"/>
-      <c r="U1" s="117"/>
-      <c r="V1" s="117"/>
-      <c r="W1" s="117"/>
-      <c r="X1" s="117"/>
-      <c r="Y1" s="117"/>
-      <c r="Z1" s="117"/>
+      <c r="R1" s="119"/>
+      <c r="S1" s="119"/>
+      <c r="T1" s="119"/>
+      <c r="U1" s="119"/>
+      <c r="V1" s="119"/>
+      <c r="W1" s="119"/>
+      <c r="X1" s="119"/>
+      <c r="Y1" s="119"/>
+      <c r="Z1" s="119"/>
     </row>
     <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B2" s="100" t="s">
@@ -1813,28 +1809,28 @@
       <c r="D2" s="18"/>
       <c r="E2" s="19"/>
       <c r="F2" s="18"/>
-      <c r="I2" s="118" t="s">
+      <c r="I2" s="120" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="119"/>
-      <c r="K2" s="119"/>
-      <c r="L2" s="119"/>
-      <c r="M2" s="119"/>
-      <c r="N2" s="119"/>
-      <c r="O2" s="119"/>
+      <c r="J2" s="121"/>
+      <c r="K2" s="121"/>
+      <c r="L2" s="121"/>
+      <c r="M2" s="121"/>
+      <c r="N2" s="121"/>
+      <c r="O2" s="121"/>
       <c r="P2" s="20"/>
-      <c r="Q2" s="114">
+      <c r="Q2" s="116">
         <v>1</v>
       </c>
-      <c r="R2" s="115"/>
-      <c r="S2" s="115"/>
-      <c r="T2" s="115"/>
-      <c r="U2" s="115"/>
-      <c r="V2" s="115"/>
-      <c r="W2" s="115"/>
-      <c r="X2" s="115"/>
-      <c r="Y2" s="115"/>
-      <c r="Z2" s="115"/>
+      <c r="R2" s="117"/>
+      <c r="S2" s="117"/>
+      <c r="T2" s="117"/>
+      <c r="U2" s="117"/>
+      <c r="V2" s="117"/>
+      <c r="W2" s="117"/>
+      <c r="X2" s="117"/>
+      <c r="Y2" s="117"/>
+      <c r="Z2" s="117"/>
     </row>
     <row r="3" spans="1:64" s="22" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
@@ -1846,102 +1842,102 @@
       <c r="A4" s="14"/>
       <c r="B4" s="25"/>
       <c r="E4" s="26"/>
-      <c r="I4" s="111">
+      <c r="I4" s="125">
         <f>I5</f>
         <v>45810</v>
       </c>
-      <c r="J4" s="109"/>
-      <c r="K4" s="109"/>
-      <c r="L4" s="109"/>
-      <c r="M4" s="109"/>
-      <c r="N4" s="109"/>
-      <c r="O4" s="109"/>
-      <c r="P4" s="109">
+      <c r="J4" s="123"/>
+      <c r="K4" s="123"/>
+      <c r="L4" s="123"/>
+      <c r="M4" s="123"/>
+      <c r="N4" s="123"/>
+      <c r="O4" s="123"/>
+      <c r="P4" s="123">
         <f>P5</f>
         <v>45817</v>
       </c>
-      <c r="Q4" s="109"/>
-      <c r="R4" s="109"/>
-      <c r="S4" s="109"/>
-      <c r="T4" s="109"/>
-      <c r="U4" s="109"/>
-      <c r="V4" s="109"/>
-      <c r="W4" s="109">
+      <c r="Q4" s="123"/>
+      <c r="R4" s="123"/>
+      <c r="S4" s="123"/>
+      <c r="T4" s="123"/>
+      <c r="U4" s="123"/>
+      <c r="V4" s="123"/>
+      <c r="W4" s="123">
         <f>W5</f>
         <v>45824</v>
       </c>
-      <c r="X4" s="109"/>
-      <c r="Y4" s="109"/>
-      <c r="Z4" s="109"/>
-      <c r="AA4" s="109"/>
-      <c r="AB4" s="109"/>
-      <c r="AC4" s="109"/>
-      <c r="AD4" s="109">
+      <c r="X4" s="123"/>
+      <c r="Y4" s="123"/>
+      <c r="Z4" s="123"/>
+      <c r="AA4" s="123"/>
+      <c r="AB4" s="123"/>
+      <c r="AC4" s="123"/>
+      <c r="AD4" s="123">
         <f>AD5</f>
         <v>45831</v>
       </c>
-      <c r="AE4" s="109"/>
-      <c r="AF4" s="109"/>
-      <c r="AG4" s="109"/>
-      <c r="AH4" s="109"/>
-      <c r="AI4" s="109"/>
-      <c r="AJ4" s="109"/>
-      <c r="AK4" s="109">
+      <c r="AE4" s="123"/>
+      <c r="AF4" s="123"/>
+      <c r="AG4" s="123"/>
+      <c r="AH4" s="123"/>
+      <c r="AI4" s="123"/>
+      <c r="AJ4" s="123"/>
+      <c r="AK4" s="123">
         <f>AK5</f>
         <v>45838</v>
       </c>
-      <c r="AL4" s="109"/>
-      <c r="AM4" s="109"/>
-      <c r="AN4" s="109"/>
-      <c r="AO4" s="109"/>
-      <c r="AP4" s="109"/>
-      <c r="AQ4" s="109"/>
-      <c r="AR4" s="109">
+      <c r="AL4" s="123"/>
+      <c r="AM4" s="123"/>
+      <c r="AN4" s="123"/>
+      <c r="AO4" s="123"/>
+      <c r="AP4" s="123"/>
+      <c r="AQ4" s="123"/>
+      <c r="AR4" s="123">
         <f>AR5</f>
         <v>45845</v>
       </c>
-      <c r="AS4" s="109"/>
-      <c r="AT4" s="109"/>
-      <c r="AU4" s="109"/>
-      <c r="AV4" s="109"/>
-      <c r="AW4" s="109"/>
-      <c r="AX4" s="109"/>
-      <c r="AY4" s="109">
+      <c r="AS4" s="123"/>
+      <c r="AT4" s="123"/>
+      <c r="AU4" s="123"/>
+      <c r="AV4" s="123"/>
+      <c r="AW4" s="123"/>
+      <c r="AX4" s="123"/>
+      <c r="AY4" s="123">
         <f>AY5</f>
         <v>45852</v>
       </c>
-      <c r="AZ4" s="109"/>
-      <c r="BA4" s="109"/>
-      <c r="BB4" s="109"/>
-      <c r="BC4" s="109"/>
-      <c r="BD4" s="109"/>
-      <c r="BE4" s="109"/>
-      <c r="BF4" s="109">
+      <c r="AZ4" s="123"/>
+      <c r="BA4" s="123"/>
+      <c r="BB4" s="123"/>
+      <c r="BC4" s="123"/>
+      <c r="BD4" s="123"/>
+      <c r="BE4" s="123"/>
+      <c r="BF4" s="123">
         <f>BF5</f>
         <v>45859</v>
       </c>
-      <c r="BG4" s="109"/>
-      <c r="BH4" s="109"/>
-      <c r="BI4" s="109"/>
-      <c r="BJ4" s="109"/>
-      <c r="BK4" s="109"/>
-      <c r="BL4" s="110"/>
+      <c r="BG4" s="123"/>
+      <c r="BH4" s="123"/>
+      <c r="BI4" s="123"/>
+      <c r="BJ4" s="123"/>
+      <c r="BK4" s="123"/>
+      <c r="BL4" s="124"/>
     </row>
     <row r="5" spans="1:64" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="121"/>
-      <c r="B5" s="122" t="s">
+      <c r="A5" s="109"/>
+      <c r="B5" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="124" t="s">
+      <c r="C5" s="112" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="112" t="s">
+      <c r="D5" s="114" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="112" t="s">
+      <c r="E5" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="112" t="s">
+      <c r="F5" s="114" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="27">
@@ -2170,12 +2166,12 @@
       </c>
     </row>
     <row r="6" spans="1:64" s="22" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="121"/>
-      <c r="B6" s="123"/>
-      <c r="C6" s="125"/>
-      <c r="D6" s="113"/>
-      <c r="E6" s="113"/>
-      <c r="F6" s="113"/>
+      <c r="A6" s="109"/>
+      <c r="B6" s="111"/>
+      <c r="C6" s="113"/>
+      <c r="D6" s="115"/>
+      <c r="E6" s="115"/>
+      <c r="F6" s="115"/>
       <c r="I6" s="30" t="str">
         <f t="shared" ref="I6:AN6" si="3">LEFT(TEXT(I5,"ddd"),1)</f>
         <v>M</v>
@@ -3431,7 +3427,7 @@
         <v>46</v>
       </c>
       <c r="D21" s="63">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="E21" s="96">
         <v>45838</v>
@@ -3510,7 +3506,7 @@
         <v>48</v>
       </c>
       <c r="D22" s="63">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="E22" s="96">
         <v>45844</v>
@@ -3589,7 +3585,7 @@
         <v>46</v>
       </c>
       <c r="D23" s="63">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="E23" s="96">
         <v>45851</v>
@@ -3668,7 +3664,7 @@
         <v>46</v>
       </c>
       <c r="D24" s="63">
-        <v>0.33</v>
+        <v>0.66</v>
       </c>
       <c r="E24" s="96">
         <v>45856</v>
@@ -4508,17 +4504,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="Q1:Z1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="B1:F1"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
@@ -4527,6 +4512,17 @@
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="Q1:Z1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D34">
     <cfRule type="dataBar" priority="23">
@@ -4751,35 +4747,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="28" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="60f5a4f2d2b0abadcf532d48ebf9cb71">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7dd78129e6a1811f84807ad11c651531" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5091,10 +5058,52 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2348D59-3426-404A-A0C5-6456F6613EDB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5119,22 +5128,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2348D59-3426-404A-A0C5-6456F6613EDB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
finalised model testing and hyperparameter tuning, removed tableau dir, updated gantt chart
</commit_message>
<xml_diff>
--- a/documents/Gantt chart.xlsx
+++ b/documents/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alisu\OneDrive\UoB\Data Science Project\MScProject2025-Ali-Suhail\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472B5602-26CD-4C43-A521-B84F06392F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394410FB-5B47-41A9-BAAB-FA6B736607B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-3750" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1105,20 +1105,14 @@
     <xf numFmtId="169" fontId="17" fillId="5" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="167" fontId="17" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1139,14 +1133,20 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="17" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="17" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="17" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1748,8 +1748,8 @@
   </sheetPr>
   <dimension ref="A1:BL37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A11" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="BB23" sqref="BA23:BB23"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1767,37 +1767,37 @@
   <sheetData>
     <row r="1" spans="1:64" ht="53.4" customHeight="1" x14ac:dyDescent="0.8">
       <c r="A1" s="14"/>
-      <c r="B1" s="122" t="s">
+      <c r="B1" s="120" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="120" t="s">
+      <c r="I1" s="118" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="121"/>
-      <c r="K1" s="121"/>
-      <c r="L1" s="121"/>
-      <c r="M1" s="121"/>
-      <c r="N1" s="121"/>
-      <c r="O1" s="121"/>
+      <c r="J1" s="119"/>
+      <c r="K1" s="119"/>
+      <c r="L1" s="119"/>
+      <c r="M1" s="119"/>
+      <c r="N1" s="119"/>
+      <c r="O1" s="119"/>
       <c r="P1" s="20"/>
-      <c r="Q1" s="118">
+      <c r="Q1" s="116">
         <f>DATE(2025, 6, 2)</f>
         <v>45810</v>
       </c>
-      <c r="R1" s="119"/>
-      <c r="S1" s="119"/>
-      <c r="T1" s="119"/>
-      <c r="U1" s="119"/>
-      <c r="V1" s="119"/>
-      <c r="W1" s="119"/>
-      <c r="X1" s="119"/>
-      <c r="Y1" s="119"/>
-      <c r="Z1" s="119"/>
+      <c r="R1" s="117"/>
+      <c r="S1" s="117"/>
+      <c r="T1" s="117"/>
+      <c r="U1" s="117"/>
+      <c r="V1" s="117"/>
+      <c r="W1" s="117"/>
+      <c r="X1" s="117"/>
+      <c r="Y1" s="117"/>
+      <c r="Z1" s="117"/>
     </row>
     <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B2" s="100" t="s">
@@ -1809,28 +1809,28 @@
       <c r="D2" s="18"/>
       <c r="E2" s="19"/>
       <c r="F2" s="18"/>
-      <c r="I2" s="120" t="s">
+      <c r="I2" s="118" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="121"/>
-      <c r="K2" s="121"/>
-      <c r="L2" s="121"/>
-      <c r="M2" s="121"/>
-      <c r="N2" s="121"/>
-      <c r="O2" s="121"/>
+      <c r="J2" s="119"/>
+      <c r="K2" s="119"/>
+      <c r="L2" s="119"/>
+      <c r="M2" s="119"/>
+      <c r="N2" s="119"/>
+      <c r="O2" s="119"/>
       <c r="P2" s="20"/>
-      <c r="Q2" s="116">
+      <c r="Q2" s="114">
         <v>1</v>
       </c>
-      <c r="R2" s="117"/>
-      <c r="S2" s="117"/>
-      <c r="T2" s="117"/>
-      <c r="U2" s="117"/>
-      <c r="V2" s="117"/>
-      <c r="W2" s="117"/>
-      <c r="X2" s="117"/>
-      <c r="Y2" s="117"/>
-      <c r="Z2" s="117"/>
+      <c r="R2" s="115"/>
+      <c r="S2" s="115"/>
+      <c r="T2" s="115"/>
+      <c r="U2" s="115"/>
+      <c r="V2" s="115"/>
+      <c r="W2" s="115"/>
+      <c r="X2" s="115"/>
+      <c r="Y2" s="115"/>
+      <c r="Z2" s="115"/>
     </row>
     <row r="3" spans="1:64" s="22" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
@@ -1842,102 +1842,102 @@
       <c r="A4" s="14"/>
       <c r="B4" s="25"/>
       <c r="E4" s="26"/>
-      <c r="I4" s="125">
+      <c r="I4" s="111">
         <f>I5</f>
         <v>45810</v>
       </c>
-      <c r="J4" s="123"/>
-      <c r="K4" s="123"/>
-      <c r="L4" s="123"/>
-      <c r="M4" s="123"/>
-      <c r="N4" s="123"/>
-      <c r="O4" s="123"/>
-      <c r="P4" s="123">
+      <c r="J4" s="109"/>
+      <c r="K4" s="109"/>
+      <c r="L4" s="109"/>
+      <c r="M4" s="109"/>
+      <c r="N4" s="109"/>
+      <c r="O4" s="109"/>
+      <c r="P4" s="109">
         <f>P5</f>
         <v>45817</v>
       </c>
-      <c r="Q4" s="123"/>
-      <c r="R4" s="123"/>
-      <c r="S4" s="123"/>
-      <c r="T4" s="123"/>
-      <c r="U4" s="123"/>
-      <c r="V4" s="123"/>
-      <c r="W4" s="123">
+      <c r="Q4" s="109"/>
+      <c r="R4" s="109"/>
+      <c r="S4" s="109"/>
+      <c r="T4" s="109"/>
+      <c r="U4" s="109"/>
+      <c r="V4" s="109"/>
+      <c r="W4" s="109">
         <f>W5</f>
         <v>45824</v>
       </c>
-      <c r="X4" s="123"/>
-      <c r="Y4" s="123"/>
-      <c r="Z4" s="123"/>
-      <c r="AA4" s="123"/>
-      <c r="AB4" s="123"/>
-      <c r="AC4" s="123"/>
-      <c r="AD4" s="123">
+      <c r="X4" s="109"/>
+      <c r="Y4" s="109"/>
+      <c r="Z4" s="109"/>
+      <c r="AA4" s="109"/>
+      <c r="AB4" s="109"/>
+      <c r="AC4" s="109"/>
+      <c r="AD4" s="109">
         <f>AD5</f>
         <v>45831</v>
       </c>
-      <c r="AE4" s="123"/>
-      <c r="AF4" s="123"/>
-      <c r="AG4" s="123"/>
-      <c r="AH4" s="123"/>
-      <c r="AI4" s="123"/>
-      <c r="AJ4" s="123"/>
-      <c r="AK4" s="123">
+      <c r="AE4" s="109"/>
+      <c r="AF4" s="109"/>
+      <c r="AG4" s="109"/>
+      <c r="AH4" s="109"/>
+      <c r="AI4" s="109"/>
+      <c r="AJ4" s="109"/>
+      <c r="AK4" s="109">
         <f>AK5</f>
         <v>45838</v>
       </c>
-      <c r="AL4" s="123"/>
-      <c r="AM4" s="123"/>
-      <c r="AN4" s="123"/>
-      <c r="AO4" s="123"/>
-      <c r="AP4" s="123"/>
-      <c r="AQ4" s="123"/>
-      <c r="AR4" s="123">
+      <c r="AL4" s="109"/>
+      <c r="AM4" s="109"/>
+      <c r="AN4" s="109"/>
+      <c r="AO4" s="109"/>
+      <c r="AP4" s="109"/>
+      <c r="AQ4" s="109"/>
+      <c r="AR4" s="109">
         <f>AR5</f>
         <v>45845</v>
       </c>
-      <c r="AS4" s="123"/>
-      <c r="AT4" s="123"/>
-      <c r="AU4" s="123"/>
-      <c r="AV4" s="123"/>
-      <c r="AW4" s="123"/>
-      <c r="AX4" s="123"/>
-      <c r="AY4" s="123">
+      <c r="AS4" s="109"/>
+      <c r="AT4" s="109"/>
+      <c r="AU4" s="109"/>
+      <c r="AV4" s="109"/>
+      <c r="AW4" s="109"/>
+      <c r="AX4" s="109"/>
+      <c r="AY4" s="109">
         <f>AY5</f>
         <v>45852</v>
       </c>
-      <c r="AZ4" s="123"/>
-      <c r="BA4" s="123"/>
-      <c r="BB4" s="123"/>
-      <c r="BC4" s="123"/>
-      <c r="BD4" s="123"/>
-      <c r="BE4" s="123"/>
-      <c r="BF4" s="123">
+      <c r="AZ4" s="109"/>
+      <c r="BA4" s="109"/>
+      <c r="BB4" s="109"/>
+      <c r="BC4" s="109"/>
+      <c r="BD4" s="109"/>
+      <c r="BE4" s="109"/>
+      <c r="BF4" s="109">
         <f>BF5</f>
         <v>45859</v>
       </c>
-      <c r="BG4" s="123"/>
-      <c r="BH4" s="123"/>
-      <c r="BI4" s="123"/>
-      <c r="BJ4" s="123"/>
-      <c r="BK4" s="123"/>
-      <c r="BL4" s="124"/>
+      <c r="BG4" s="109"/>
+      <c r="BH4" s="109"/>
+      <c r="BI4" s="109"/>
+      <c r="BJ4" s="109"/>
+      <c r="BK4" s="109"/>
+      <c r="BL4" s="110"/>
     </row>
     <row r="5" spans="1:64" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="109"/>
-      <c r="B5" s="110" t="s">
+      <c r="A5" s="121"/>
+      <c r="B5" s="122" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="112" t="s">
+      <c r="C5" s="124" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="114" t="s">
+      <c r="D5" s="112" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="114" t="s">
+      <c r="E5" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="114" t="s">
+      <c r="F5" s="112" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="27">
@@ -2166,12 +2166,12 @@
       </c>
     </row>
     <row r="6" spans="1:64" s="22" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="109"/>
-      <c r="B6" s="111"/>
-      <c r="C6" s="113"/>
-      <c r="D6" s="115"/>
-      <c r="E6" s="115"/>
-      <c r="F6" s="115"/>
+      <c r="A6" s="121"/>
+      <c r="B6" s="123"/>
+      <c r="C6" s="125"/>
+      <c r="D6" s="113"/>
+      <c r="E6" s="113"/>
+      <c r="F6" s="113"/>
       <c r="I6" s="30" t="str">
         <f t="shared" ref="I6:AN6" si="3">LEFT(TEXT(I5,"ddd"),1)</f>
         <v>M</v>
@@ -3585,7 +3585,7 @@
         <v>46</v>
       </c>
       <c r="D23" s="63">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="E23" s="96">
         <v>45851</v>
@@ -3664,7 +3664,7 @@
         <v>46</v>
       </c>
       <c r="D24" s="63">
-        <v>0.66</v>
+        <v>0.9</v>
       </c>
       <c r="E24" s="96">
         <v>45856</v>
@@ -4504,6 +4504,17 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="Q1:Z1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="B1:F1"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
@@ -4512,17 +4523,6 @@
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="Q1:Z1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D34">
     <cfRule type="dataBar" priority="23">
@@ -4747,6 +4747,35 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="28" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="60f5a4f2d2b0abadcf532d48ebf9cb71">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7dd78129e6a1811f84807ad11c651531" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5058,52 +5087,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2348D59-3426-404A-A0C5-6456F6613EDB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5128,9 +5115,22 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2348D59-3426-404A-A0C5-6456F6613EDB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Added hypothesis tests, RBF model implemented, tuned and evaluated, updated gantt chart, added report structure draft and report drafts, almost finished methods section of the report, added img dir for report plots.
</commit_message>
<xml_diff>
--- a/documents/Gantt chart.xlsx
+++ b/documents/Gantt chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alisu\OneDrive\UoB\Data Science Project\MScProject2025-Ali-Suhail\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/425b9db2548ee741/UoB/Data Science Project/MScProject2025-Ali-Suhail/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394410FB-5B47-41A9-BAAB-FA6B736607B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{90722E1F-2930-4829-963F-D550B1B4DBE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E128E0C8-CB1A-4402-9941-399E5BAEDB55}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-3750" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project schedule" sheetId="11" r:id="rId1"/>
@@ -1748,8 +1748,8 @@
   </sheetPr>
   <dimension ref="A1:BL37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A23" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3506,7 +3506,7 @@
         <v>48</v>
       </c>
       <c r="D22" s="63">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E22" s="96">
         <v>45844</v>
@@ -3664,7 +3664,7 @@
         <v>46</v>
       </c>
       <c r="D24" s="63">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E24" s="96">
         <v>45856</v>
@@ -3969,7 +3969,7 @@
         <v>46</v>
       </c>
       <c r="D28" s="70">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E28" s="99">
         <v>45870</v>
@@ -4747,15 +4747,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -4775,7 +4766,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="28" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="60f5a4f2d2b0abadcf532d48ebf9cb71">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7dd78129e6a1811f84807ad11c651531" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5087,15 +5078,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -5114,7 +5106,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2348D59-3426-404A-A0C5-6456F6613EDB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5135,6 +5127,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>

<commit_message>
removed old dir from codes, plot format changes in models.ipynb, updated gantt chart and added report drafts and presentation drafts, added kanban board dump, removed irrelevent files/dirs
</commit_message>
<xml_diff>
--- a/documents/Gantt chart.xlsx
+++ b/documents/Gantt chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/425b9db2548ee741/UoB/Data Science Project/MScProject2025-Ali-Suhail/documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alisu\OneDrive\UoB\Data Science Project\MScProject2025-Ali-Suhail\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{90722E1F-2930-4829-963F-D550B1B4DBE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E128E0C8-CB1A-4402-9941-399E5BAEDB55}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F819BB-FFD3-485F-9986-38A7AC22E04C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-3750" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project schedule" sheetId="11" r:id="rId1"/>
@@ -1105,14 +1105,20 @@
     <xf numFmtId="169" fontId="17" fillId="5" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="17" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="17" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="17" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1133,20 +1139,14 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="167" fontId="17" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1748,8 +1748,8 @@
   </sheetPr>
   <dimension ref="A1:BL37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A23" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2:Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1767,37 +1767,37 @@
   <sheetData>
     <row r="1" spans="1:64" ht="53.4" customHeight="1" x14ac:dyDescent="0.8">
       <c r="A1" s="14"/>
-      <c r="B1" s="120" t="s">
+      <c r="B1" s="122" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="118" t="s">
+      <c r="I1" s="120" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="119"/>
-      <c r="K1" s="119"/>
-      <c r="L1" s="119"/>
-      <c r="M1" s="119"/>
-      <c r="N1" s="119"/>
-      <c r="O1" s="119"/>
+      <c r="J1" s="121"/>
+      <c r="K1" s="121"/>
+      <c r="L1" s="121"/>
+      <c r="M1" s="121"/>
+      <c r="N1" s="121"/>
+      <c r="O1" s="121"/>
       <c r="P1" s="20"/>
-      <c r="Q1" s="116">
+      <c r="Q1" s="118">
         <f>DATE(2025, 6, 2)</f>
         <v>45810</v>
       </c>
-      <c r="R1" s="117"/>
-      <c r="S1" s="117"/>
-      <c r="T1" s="117"/>
-      <c r="U1" s="117"/>
-      <c r="V1" s="117"/>
-      <c r="W1" s="117"/>
-      <c r="X1" s="117"/>
-      <c r="Y1" s="117"/>
-      <c r="Z1" s="117"/>
+      <c r="R1" s="119"/>
+      <c r="S1" s="119"/>
+      <c r="T1" s="119"/>
+      <c r="U1" s="119"/>
+      <c r="V1" s="119"/>
+      <c r="W1" s="119"/>
+      <c r="X1" s="119"/>
+      <c r="Y1" s="119"/>
+      <c r="Z1" s="119"/>
     </row>
     <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B2" s="100" t="s">
@@ -1809,28 +1809,28 @@
       <c r="D2" s="18"/>
       <c r="E2" s="19"/>
       <c r="F2" s="18"/>
-      <c r="I2" s="118" t="s">
+      <c r="I2" s="120" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="119"/>
-      <c r="K2" s="119"/>
-      <c r="L2" s="119"/>
-      <c r="M2" s="119"/>
-      <c r="N2" s="119"/>
-      <c r="O2" s="119"/>
+      <c r="J2" s="121"/>
+      <c r="K2" s="121"/>
+      <c r="L2" s="121"/>
+      <c r="M2" s="121"/>
+      <c r="N2" s="121"/>
+      <c r="O2" s="121"/>
       <c r="P2" s="20"/>
-      <c r="Q2" s="114">
+      <c r="Q2" s="116">
         <v>1</v>
       </c>
-      <c r="R2" s="115"/>
-      <c r="S2" s="115"/>
-      <c r="T2" s="115"/>
-      <c r="U2" s="115"/>
-      <c r="V2" s="115"/>
-      <c r="W2" s="115"/>
-      <c r="X2" s="115"/>
-      <c r="Y2" s="115"/>
-      <c r="Z2" s="115"/>
+      <c r="R2" s="117"/>
+      <c r="S2" s="117"/>
+      <c r="T2" s="117"/>
+      <c r="U2" s="117"/>
+      <c r="V2" s="117"/>
+      <c r="W2" s="117"/>
+      <c r="X2" s="117"/>
+      <c r="Y2" s="117"/>
+      <c r="Z2" s="117"/>
     </row>
     <row r="3" spans="1:64" s="22" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
@@ -1842,102 +1842,102 @@
       <c r="A4" s="14"/>
       <c r="B4" s="25"/>
       <c r="E4" s="26"/>
-      <c r="I4" s="111">
+      <c r="I4" s="125">
         <f>I5</f>
         <v>45810</v>
       </c>
-      <c r="J4" s="109"/>
-      <c r="K4" s="109"/>
-      <c r="L4" s="109"/>
-      <c r="M4" s="109"/>
-      <c r="N4" s="109"/>
-      <c r="O4" s="109"/>
-      <c r="P4" s="109">
+      <c r="J4" s="123"/>
+      <c r="K4" s="123"/>
+      <c r="L4" s="123"/>
+      <c r="M4" s="123"/>
+      <c r="N4" s="123"/>
+      <c r="O4" s="123"/>
+      <c r="P4" s="123">
         <f>P5</f>
         <v>45817</v>
       </c>
-      <c r="Q4" s="109"/>
-      <c r="R4" s="109"/>
-      <c r="S4" s="109"/>
-      <c r="T4" s="109"/>
-      <c r="U4" s="109"/>
-      <c r="V4" s="109"/>
-      <c r="W4" s="109">
+      <c r="Q4" s="123"/>
+      <c r="R4" s="123"/>
+      <c r="S4" s="123"/>
+      <c r="T4" s="123"/>
+      <c r="U4" s="123"/>
+      <c r="V4" s="123"/>
+      <c r="W4" s="123">
         <f>W5</f>
         <v>45824</v>
       </c>
-      <c r="X4" s="109"/>
-      <c r="Y4" s="109"/>
-      <c r="Z4" s="109"/>
-      <c r="AA4" s="109"/>
-      <c r="AB4" s="109"/>
-      <c r="AC4" s="109"/>
-      <c r="AD4" s="109">
+      <c r="X4" s="123"/>
+      <c r="Y4" s="123"/>
+      <c r="Z4" s="123"/>
+      <c r="AA4" s="123"/>
+      <c r="AB4" s="123"/>
+      <c r="AC4" s="123"/>
+      <c r="AD4" s="123">
         <f>AD5</f>
         <v>45831</v>
       </c>
-      <c r="AE4" s="109"/>
-      <c r="AF4" s="109"/>
-      <c r="AG4" s="109"/>
-      <c r="AH4" s="109"/>
-      <c r="AI4" s="109"/>
-      <c r="AJ4" s="109"/>
-      <c r="AK4" s="109">
+      <c r="AE4" s="123"/>
+      <c r="AF4" s="123"/>
+      <c r="AG4" s="123"/>
+      <c r="AH4" s="123"/>
+      <c r="AI4" s="123"/>
+      <c r="AJ4" s="123"/>
+      <c r="AK4" s="123">
         <f>AK5</f>
         <v>45838</v>
       </c>
-      <c r="AL4" s="109"/>
-      <c r="AM4" s="109"/>
-      <c r="AN4" s="109"/>
-      <c r="AO4" s="109"/>
-      <c r="AP4" s="109"/>
-      <c r="AQ4" s="109"/>
-      <c r="AR4" s="109">
+      <c r="AL4" s="123"/>
+      <c r="AM4" s="123"/>
+      <c r="AN4" s="123"/>
+      <c r="AO4" s="123"/>
+      <c r="AP4" s="123"/>
+      <c r="AQ4" s="123"/>
+      <c r="AR4" s="123">
         <f>AR5</f>
         <v>45845</v>
       </c>
-      <c r="AS4" s="109"/>
-      <c r="AT4" s="109"/>
-      <c r="AU4" s="109"/>
-      <c r="AV4" s="109"/>
-      <c r="AW4" s="109"/>
-      <c r="AX4" s="109"/>
-      <c r="AY4" s="109">
+      <c r="AS4" s="123"/>
+      <c r="AT4" s="123"/>
+      <c r="AU4" s="123"/>
+      <c r="AV4" s="123"/>
+      <c r="AW4" s="123"/>
+      <c r="AX4" s="123"/>
+      <c r="AY4" s="123">
         <f>AY5</f>
         <v>45852</v>
       </c>
-      <c r="AZ4" s="109"/>
-      <c r="BA4" s="109"/>
-      <c r="BB4" s="109"/>
-      <c r="BC4" s="109"/>
-      <c r="BD4" s="109"/>
-      <c r="BE4" s="109"/>
-      <c r="BF4" s="109">
+      <c r="AZ4" s="123"/>
+      <c r="BA4" s="123"/>
+      <c r="BB4" s="123"/>
+      <c r="BC4" s="123"/>
+      <c r="BD4" s="123"/>
+      <c r="BE4" s="123"/>
+      <c r="BF4" s="123">
         <f>BF5</f>
         <v>45859</v>
       </c>
-      <c r="BG4" s="109"/>
-      <c r="BH4" s="109"/>
-      <c r="BI4" s="109"/>
-      <c r="BJ4" s="109"/>
-      <c r="BK4" s="109"/>
-      <c r="BL4" s="110"/>
+      <c r="BG4" s="123"/>
+      <c r="BH4" s="123"/>
+      <c r="BI4" s="123"/>
+      <c r="BJ4" s="123"/>
+      <c r="BK4" s="123"/>
+      <c r="BL4" s="124"/>
     </row>
     <row r="5" spans="1:64" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="121"/>
-      <c r="B5" s="122" t="s">
+      <c r="A5" s="109"/>
+      <c r="B5" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="124" t="s">
+      <c r="C5" s="112" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="112" t="s">
+      <c r="D5" s="114" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="112" t="s">
+      <c r="E5" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="112" t="s">
+      <c r="F5" s="114" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="27">
@@ -2166,12 +2166,12 @@
       </c>
     </row>
     <row r="6" spans="1:64" s="22" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="121"/>
-      <c r="B6" s="123"/>
-      <c r="C6" s="125"/>
-      <c r="D6" s="113"/>
-      <c r="E6" s="113"/>
-      <c r="F6" s="113"/>
+      <c r="A6" s="109"/>
+      <c r="B6" s="111"/>
+      <c r="C6" s="113"/>
+      <c r="D6" s="115"/>
+      <c r="E6" s="115"/>
+      <c r="F6" s="115"/>
       <c r="I6" s="30" t="str">
         <f t="shared" ref="I6:AN6" si="3">LEFT(TEXT(I5,"ddd"),1)</f>
         <v>M</v>
@@ -3585,7 +3585,7 @@
         <v>46</v>
       </c>
       <c r="D23" s="63">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E23" s="96">
         <v>45851</v>
@@ -3890,7 +3890,7 @@
         <v>46</v>
       </c>
       <c r="D27" s="70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="99">
         <v>45863</v>
@@ -3969,7 +3969,7 @@
         <v>46</v>
       </c>
       <c r="D28" s="70">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E28" s="99">
         <v>45870</v>
@@ -4048,7 +4048,7 @@
         <v>46</v>
       </c>
       <c r="D29" s="70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" s="99">
         <v>45877</v>
@@ -4127,7 +4127,7 @@
         <v>46</v>
       </c>
       <c r="D30" s="70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" s="99">
         <v>45884</v>
@@ -4206,7 +4206,7 @@
         <v>50</v>
       </c>
       <c r="D31" s="70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" s="99">
         <v>45886</v>
@@ -4285,7 +4285,7 @@
         <v>46</v>
       </c>
       <c r="D32" s="103">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" s="104">
         <v>45891</v>
@@ -4504,17 +4504,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="Q1:Z1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="B1:F1"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
@@ -4523,6 +4512,17 @@
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="Q1:Z1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D34">
     <cfRule type="dataBar" priority="23">
@@ -4747,23 +4747,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5079,29 +5068,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5128,9 +5117,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>